<commit_message>
Grado 11 - Guion 01
ARchivos con corrección de estilo, a cargo de Gladys Peñuela
Queda pendiente comparar mapa conceptual: versión autor y versión
correctora.
</commit_message>
<xml_diff>
--- a/seguimiento/Grado11.xlsx
+++ b/seguimiento/Grado11.xlsx
@@ -26,6 +26,29 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Flor Buitrago</author>
+  </authors>
+  <commentList>
+    <comment ref="B12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>La correctora de estilo entregó los archivos completos</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
@@ -90,7 +113,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +152,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="15">
@@ -851,11 +880,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,9 +1108,15 @@
       <c r="A12" s="29">
         <v>7</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="B12" s="4">
+        <v>42091</v>
+      </c>
+      <c r="C12" s="5">
+        <v>42091</v>
+      </c>
+      <c r="D12" s="5">
+        <v>42086</v>
+      </c>
       <c r="E12" s="5"/>
       <c r="F12" s="6"/>
       <c r="G12" s="10"/>
@@ -1259,6 +1294,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>